<commit_message>
Auto stash before merge of "code" and "origin/code"
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Loyse/Journal_Travail.xlsx
+++ b/Dossiers personnels/Loyse/Journal_Travail.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Finition du Gantt, Cahier des charges, répartition des heures</t>
+  </si>
+  <si>
+    <t>Discussion de sur l'implémentation du undo-redo + établissement d'un diagramme de classe du model</t>
+  </si>
+  <si>
+    <t>Réunion de mise en commun du travail + discussion du undo-redo</t>
+  </si>
+  <si>
+    <t>Recherche sur l'implementation de la sauvegarde</t>
+  </si>
+  <si>
+    <t>test d'implémentation du système de sauvegrade par sérialisation</t>
   </si>
 </sst>
 </file>
@@ -461,7 +473,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,25 +594,49 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>43168</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>43171</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
+      <c r="A15" s="3">
+        <v>43175</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>43177</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -688,7 +724,7 @@
       </c>
       <c r="C33" s="9">
         <f>SUM(C5:C32)</f>
-        <v>12.75</v>
+        <v>25.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>